<commit_message>
Adding rest of the files worked with/on
adding new relevant files and any updates to previous files.
</commit_message>
<xml_diff>
--- a/Math353Data.xlsx
+++ b/Math353Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rickymiranda/Documents/Gettysburg College 2017-2022/Senior Year 2022/Math 353/StatsProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40149D17-5F65-F047-ABE0-8F138CD0A7AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADE4C4B-316E-0440-A16F-1AE42442C382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16460" tabRatio="786" activeTab="2" xr2:uid="{2BB882B7-595F-49B1-A03D-4CFCB859DDE8}"/>
+    <workbookView xWindow="4800" yWindow="500" windowWidth="28800" windowHeight="16460" tabRatio="786" xr2:uid="{2BB882B7-595F-49B1-A03D-4CFCB859DDE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -1116,8 +1116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D63804E-A8EC-45E0-B302-6D82E2A1CE8B}">
   <dimension ref="A1:N123"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3414,237 +3414,237 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16D76710-6324-4F05-9B43-36766291B1DB}">
-  <dimension ref="B2:F13"/>
+  <dimension ref="B1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F2"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>15</v>
+      <c r="B2" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="6">
+        <v>44</v>
+      </c>
+      <c r="D2" s="6">
+        <v>275.60000000000002</v>
+      </c>
+      <c r="E2" s="4">
+        <f>D2/(C2*2.2)</f>
+        <v>2.8471074380165287</v>
+      </c>
+      <c r="F2" s="4">
+        <f>((D2/2.2)*500) / (Data!$J$15 + Data!$J$16*C2 + Data!$J$17*C2^2 +Data!$J$18*C2^3 + Data!$J$19*C2^4 + Data!$J$20*C2^5)</f>
+        <v>176.3928506540353</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C3" s="6">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D3" s="6">
-        <v>275.60000000000002</v>
+        <v>424.4</v>
       </c>
       <c r="E3" s="4">
-        <f>D3/(C3*2.2)</f>
-        <v>2.8471074380165287</v>
+        <f t="shared" ref="E3:E12" si="0">D3/(C3*2.2)</f>
+        <v>4.0189393939393936</v>
       </c>
       <c r="F3" s="4">
         <f>((D3/2.2)*500) / (Data!$J$15 + Data!$J$16*C3 + Data!$J$17*C3^2 +Data!$J$18*C3^3 + Data!$J$19*C3^4 + Data!$J$20*C3^5)</f>
-        <v>176.3928506540353</v>
+        <v>255.4927415999245</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="C4" s="6">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D4" s="6">
-        <v>424.4</v>
+        <v>418.9</v>
       </c>
       <c r="E4" s="4">
-        <f t="shared" ref="E4:E13" si="0">D4/(C4*2.2)</f>
-        <v>4.0189393939393936</v>
+        <f t="shared" si="0"/>
+        <v>3.6617132867132862</v>
       </c>
       <c r="F4" s="4">
         <f>((D4/2.2)*500) / (Data!$J$15 + Data!$J$16*C4 + Data!$J$17*C4^2 +Data!$J$18*C4^3 + Data!$J$19*C4^4 + Data!$J$20*C4^5)</f>
-        <v>255.4927415999245</v>
+        <v>237.37101585104108</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C5" s="6">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D5" s="6">
         <v>418.9</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" si="0"/>
-        <v>3.6617132867132862</v>
+        <v>3.4001623376623371</v>
       </c>
       <c r="F5" s="4">
         <f>((D5/2.2)*500) / (Data!$J$15 + Data!$J$16*C5 + Data!$J$17*C5^2 +Data!$J$18*C5^3 + Data!$J$19*C5^4 + Data!$J$20*C5^5)</f>
-        <v>237.37101585104108</v>
+        <v>224.0363086554604</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C6" s="6">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D6" s="6">
-        <v>418.9</v>
+        <v>468.5</v>
       </c>
       <c r="E6" s="4">
         <f t="shared" si="0"/>
-        <v>3.4001623376623371</v>
+        <v>3.5492424242424243</v>
       </c>
       <c r="F6" s="4">
         <f>((D6/2.2)*500) / (Data!$J$15 + Data!$J$16*C6 + Data!$J$17*C6^2 +Data!$J$18*C6^3 + Data!$J$19*C6^4 + Data!$J$20*C6^5)</f>
-        <v>224.0363086554604</v>
+        <v>237.42022776127007</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C7" s="6">
-        <v>60</v>
+        <v>67.5</v>
       </c>
       <c r="D7" s="6">
-        <v>468.5</v>
+        <v>498.2</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" si="0"/>
-        <v>3.5492424242424243</v>
+        <v>3.354882154882155</v>
       </c>
       <c r="F7" s="4">
         <f>((D7/2.2)*500) / (Data!$J$15 + Data!$J$16*C7 + Data!$J$17*C7^2 +Data!$J$18*C7^3 + Data!$J$19*C7^4 + Data!$J$20*C7^5)</f>
-        <v>237.42022776127007</v>
+        <v>231.12435929046157</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C8" s="6">
-        <v>67.5</v>
+        <v>75</v>
       </c>
       <c r="D8" s="6">
-        <v>498.2</v>
+        <v>542.29999999999995</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
-        <v>3.354882154882155</v>
+        <v>3.2866666666666662</v>
       </c>
       <c r="F8" s="4">
         <f>((D8/2.2)*500) / (Data!$J$15 + Data!$J$16*C8 + Data!$J$17*C8^2 +Data!$J$18*C8^3 + Data!$J$19*C8^4 + Data!$J$20*C8^5)</f>
-        <v>231.12435929046157</v>
+        <v>234.33292171663294</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C9" s="6">
-        <v>75</v>
+        <v>82.5</v>
       </c>
       <c r="D9" s="6">
-        <v>542.29999999999995</v>
+        <v>468.5</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
-        <v>3.2866666666666662</v>
+        <v>2.5812672176308538</v>
       </c>
       <c r="F9" s="4">
         <f>((D9/2.2)*500) / (Data!$J$15 + Data!$J$16*C9 + Data!$J$17*C9^2 +Data!$J$18*C9^3 + Data!$J$19*C9^4 + Data!$J$20*C9^5)</f>
-        <v>234.33292171663294</v>
+        <v>191.65255825783331</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="C10" s="6">
-        <v>82.5</v>
+        <v>90</v>
       </c>
       <c r="D10" s="6">
-        <v>468.5</v>
+        <v>573.20000000000005</v>
       </c>
       <c r="E10" s="4">
         <f t="shared" si="0"/>
-        <v>2.5812672176308538</v>
+        <v>2.8949494949494947</v>
       </c>
       <c r="F10" s="4">
         <f>((D10/2.2)*500) / (Data!$J$15 + Data!$J$16*C10 + Data!$J$17*C10^2 +Data!$J$18*C10^3 + Data!$J$19*C10^4 + Data!$J$20*C10^5)</f>
-        <v>191.65255825783331</v>
+        <v>225.12802155713979</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C11" s="6">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D11" s="6">
-        <v>573.20000000000005</v>
+        <v>532.4</v>
       </c>
       <c r="E11" s="4">
         <f t="shared" si="0"/>
-        <v>2.8949494949494947</v>
+        <v>2.4199999999999995</v>
       </c>
       <c r="F11" s="4">
         <f>((D11/2.2)*500) / (Data!$J$15 + Data!$J$16*C11 + Data!$J$17*C11^2 +Data!$J$18*C11^3 + Data!$J$19*C11^4 + Data!$J$20*C11^5)</f>
-        <v>225.12802155713979</v>
+        <v>201.48516265031091</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="C12" s="6">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D12" s="6">
-        <v>532.4</v>
+        <v>573.20000000000005</v>
       </c>
       <c r="E12" s="4">
         <f t="shared" si="0"/>
-        <v>2.4199999999999995</v>
+        <v>2.368595041322314</v>
       </c>
       <c r="F12" s="4">
         <f>((D12/2.2)*500) / (Data!$J$15 + Data!$J$16*C12 + Data!$J$17*C12^2 +Data!$J$18*C12^3 + Data!$J$19*C12^4 + Data!$J$20*C12^5)</f>
-        <v>201.48516265031091</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B13" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C13" s="6">
-        <v>110</v>
-      </c>
-      <c r="D13" s="6">
-        <v>573.20000000000005</v>
-      </c>
-      <c r="E13" s="4">
-        <f t="shared" si="0"/>
-        <v>2.368595041322314</v>
-      </c>
-      <c r="F13" s="4">
-        <f>((D13/2.2)*500) / (Data!$J$15 + Data!$J$16*C13 + Data!$J$17*C13^2 +Data!$J$18*C13^3 + Data!$J$19*C13^4 + Data!$J$20*C13^5)</f>
         <v>211.84100129321362</v>
       </c>
     </row>
@@ -3655,10 +3655,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{045BE198-35E4-4C95-91AB-69F293A738FE}">
-  <dimension ref="B2:F13"/>
+  <dimension ref="B1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V31" sqref="V31"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3670,229 +3670,229 @@
     <col min="6" max="6" width="6.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>15</v>
+      <c r="B2" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="6">
+        <v>44</v>
+      </c>
+      <c r="D2" s="6">
+        <v>600.79999999999995</v>
+      </c>
+      <c r="E2" s="4">
+        <f>D2/(C2*2.2)</f>
+        <v>6.206611570247933</v>
+      </c>
+      <c r="F2" s="4">
+        <f>((D2/2.2)*500) / (Data!$J$15 + Data!$J$16*C2 + Data!$J$17*C2^2 + Data!$J$18*C2^3 + Data!$J$19*C2^4 + Data!$J$20*C2^5)</f>
+        <v>384.5312941688839</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C3" s="6">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D3" s="6">
-        <v>600.79999999999995</v>
+        <v>899.5</v>
       </c>
       <c r="E3" s="4">
-        <f>D3/(C3*2.2)</f>
-        <v>6.206611570247933</v>
+        <f t="shared" ref="E3:E12" si="0">D3/(C3*2.2)</f>
+        <v>8.5179924242424239</v>
       </c>
       <c r="F3" s="4">
         <f>((D3/2.2)*500) / (Data!$J$15 + Data!$J$16*C3 + Data!$J$17*C3^2 + Data!$J$18*C3^3 + Data!$J$19*C3^4 + Data!$J$20*C3^5)</f>
-        <v>384.5312941688839</v>
+        <v>541.50735407429795</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="C4" s="6">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D4" s="6">
-        <v>899.5</v>
+        <v>948</v>
       </c>
       <c r="E4" s="4">
-        <f t="shared" ref="E4:E13" si="0">D4/(C4*2.2)</f>
-        <v>8.5179924242424239</v>
+        <f t="shared" si="0"/>
+        <v>8.2867132867132867</v>
       </c>
       <c r="F4" s="4">
         <f>((D4/2.2)*500) / (Data!$J$15 + Data!$J$16*C4 + Data!$J$17*C4^2 + Data!$J$18*C4^3 + Data!$J$19*C4^4 + Data!$J$20*C4^5)</f>
-        <v>541.50735407429795</v>
+        <v>537.18721180899252</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="C5" s="6">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D5" s="6">
-        <v>948</v>
+        <v>983.3</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" si="0"/>
-        <v>8.2867132867132867</v>
+        <v>7.9813311688311677</v>
       </c>
       <c r="F5" s="4">
         <f>((D5/2.2)*500) / (Data!$J$15 + Data!$J$16*C5 + Data!$J$17*C5^2 + Data!$J$18*C5^3 + Data!$J$19*C5^4 + Data!$J$20*C5^5)</f>
-        <v>537.18721180899252</v>
+        <v>525.88900047962329</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="6">
         <v>60</v>
       </c>
-      <c r="C6" s="6">
-        <v>56</v>
-      </c>
       <c r="D6" s="6">
-        <v>983.3</v>
+        <v>1069.2</v>
       </c>
       <c r="E6" s="4">
         <f t="shared" si="0"/>
-        <v>7.9813311688311677</v>
+        <v>8.1</v>
       </c>
       <c r="F6" s="4">
         <f>((D6/2.2)*500) / (Data!$J$15 + Data!$J$16*C6 + Data!$J$17*C6^2 + Data!$J$18*C6^3 + Data!$J$19*C6^4 + Data!$J$20*C6^5)</f>
-        <v>525.88900047962329</v>
+        <v>541.8350213924225</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C7" s="6">
-        <v>60</v>
+        <v>67.5</v>
       </c>
       <c r="D7" s="6">
-        <v>1069.2</v>
+        <v>1135.4000000000001</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" si="0"/>
-        <v>8.1</v>
+        <v>7.645791245791246</v>
       </c>
       <c r="F7" s="4">
         <f>((D7/2.2)*500) / (Data!$J$15 + Data!$J$16*C7 + Data!$J$17*C7^2 + Data!$J$18*C7^3 + Data!$J$19*C7^4 + Data!$J$20*C7^5)</f>
-        <v>541.8350213924225</v>
+        <v>526.73343544437989</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C8" s="6">
-        <v>67.5</v>
+        <v>75</v>
       </c>
       <c r="D8" s="6">
-        <v>1135.4000000000001</v>
+        <v>1210.3</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
-        <v>7.645791245791246</v>
+        <v>7.335151515151515</v>
       </c>
       <c r="F8" s="4">
         <f>((D8/2.2)*500) / (Data!$J$15 + Data!$J$16*C8 + Data!$J$17*C8^2 + Data!$J$18*C8^3 + Data!$J$19*C8^4 + Data!$J$20*C8^5)</f>
-        <v>526.73343544437989</v>
+        <v>522.98199364492143</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C9" s="6">
-        <v>75</v>
+        <v>82.5</v>
       </c>
       <c r="D9" s="6">
-        <v>1210.3</v>
+        <v>1069.2</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
-        <v>7.335151515151515</v>
+        <v>5.8909090909090907</v>
       </c>
       <c r="F9" s="4">
         <f>((D9/2.2)*500) / (Data!$J$15 + Data!$J$16*C9 + Data!$J$17*C9^2 + Data!$J$18*C9^3 + Data!$J$19*C9^4 + Data!$J$20*C9^5)</f>
-        <v>522.98199364492143</v>
+        <v>437.38509133249812</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="C10" s="6">
-        <v>82.5</v>
+        <v>90</v>
       </c>
       <c r="D10" s="6">
-        <v>1069.2</v>
+        <v>1424.2</v>
       </c>
       <c r="E10" s="4">
         <f t="shared" si="0"/>
-        <v>5.8909090909090907</v>
+        <v>7.1929292929292918</v>
       </c>
       <c r="F10" s="4">
         <f>((D10/2.2)*500) / (Data!$J$15 + Data!$J$16*C10 + Data!$J$17*C10^2 + Data!$J$18*C10^3 + Data!$J$19*C10^4 + Data!$J$20*C10^5)</f>
-        <v>437.38509133249812</v>
+        <v>559.36379675798753</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C11" s="6">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D11" s="6">
-        <v>1424.2</v>
+        <v>1232.4000000000001</v>
       </c>
       <c r="E11" s="4">
         <f t="shared" si="0"/>
-        <v>7.1929292929292918</v>
+        <v>5.6018181818181816</v>
       </c>
       <c r="F11" s="4">
         <f>((D11/2.2)*500) / (Data!$J$15 + Data!$J$16*C11 + Data!$J$17*C11^2 + Data!$J$18*C11^3 + Data!$J$19*C11^4 + Data!$J$20*C11^5)</f>
-        <v>559.36379675798753</v>
+        <v>466.3980361574815</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C12" s="6">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D12" s="6">
-        <v>1232.4000000000001</v>
+        <v>1480.4</v>
       </c>
       <c r="E12" s="4">
         <f t="shared" si="0"/>
-        <v>5.6018181818181816</v>
+        <v>6.1173553719008265</v>
       </c>
       <c r="F12" s="4">
         <f>((D12/2.2)*500) / (Data!$J$15 + Data!$J$16*C12 + Data!$J$17*C12^2 + Data!$J$18*C12^3 + Data!$J$19*C12^4 + Data!$J$20*C12^5)</f>
-        <v>466.3980361574815</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B13" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C13" s="6">
-        <v>110</v>
-      </c>
-      <c r="D13" s="6">
-        <v>1480.4</v>
-      </c>
-      <c r="E13" s="4">
-        <f t="shared" si="0"/>
-        <v>6.1173553719008265</v>
-      </c>
-      <c r="F13" s="4">
-        <f>((D13/2.2)*500) / (Data!$J$15 + Data!$J$16*C13 + Data!$J$17*C13^2 + Data!$J$18*C13^3 + Data!$J$19*C13^4 + Data!$J$20*C13^5)</f>
         <v>547.12040878310086</v>
       </c>
     </row>
@@ -3906,7 +3906,7 @@
   <dimension ref="B1:K85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="H1" sqref="H1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7150,7 +7150,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3360F033-907C-4E12-8507-1910F4CF6D65}">
   <dimension ref="B1:K83"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="103" workbookViewId="0">
+    <sheetView zoomScale="103" workbookViewId="0">
       <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
@@ -10060,10 +10060,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E8E5A40-B044-4545-B236-178F265A3E95}">
-  <dimension ref="B2:F14"/>
+  <dimension ref="B1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10075,248 +10075,248 @@
     <col min="6" max="6" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>15</v>
+        <v>1</v>
+      </c>
+      <c r="C2" s="6">
+        <v>52</v>
+      </c>
+      <c r="D2" s="6">
+        <v>363.8</v>
+      </c>
+      <c r="E2" s="4">
+        <f>D2/(C2*2.2)</f>
+        <v>3.18006993006993</v>
+      </c>
+      <c r="F2" s="4">
+        <f>((D2/2.2)*500) / (Data!$J$8 + Data!$J$9*C2 + Data!$J$10*C2^2 + Data!$J$11*C2^3 + Data!$J$12*C2^4 + Data!$J$13*C2^5)</f>
+        <v>162.26777647722309</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" s="6">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D3" s="6">
-        <v>363.8</v>
+        <v>385.8</v>
       </c>
       <c r="E3" s="4">
-        <f>D3/(C3*2.2)</f>
-        <v>3.18006993006993</v>
+        <f t="shared" ref="E3:E13" si="0">D3/(C3*2.2)</f>
+        <v>3.1314935064935061</v>
       </c>
       <c r="F3" s="4">
         <f>((D3/2.2)*500) / (Data!$J$8 + Data!$J$9*C3 + Data!$J$10*C3^2 + Data!$J$11*C3^3 + Data!$J$12*C3^4 + Data!$J$13*C3^5)</f>
-        <v>162.26777647722309</v>
+        <v>159.6419834876825</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" s="6">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D4" s="6">
-        <v>385.8</v>
+        <v>535.70000000000005</v>
       </c>
       <c r="E4" s="4">
-        <f t="shared" ref="E4:E14" si="0">D4/(C4*2.2)</f>
-        <v>3.1314935064935061</v>
+        <f t="shared" si="0"/>
+        <v>4.0583333333333336</v>
       </c>
       <c r="F4" s="4">
         <f>((D4/2.2)*500) / (Data!$J$8 + Data!$J$9*C4 + Data!$J$10*C4^2 + Data!$J$11*C4^3 + Data!$J$12*C4^4 + Data!$J$13*C4^5)</f>
-        <v>159.6419834876825</v>
+        <v>207.67487661192092</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5" s="6">
-        <v>60</v>
+        <v>67.5</v>
       </c>
       <c r="D5" s="6">
-        <v>535.70000000000005</v>
+        <v>583.1</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" si="0"/>
-        <v>4.0583333333333336</v>
+        <v>3.9265993265993266</v>
       </c>
       <c r="F5" s="4">
         <f>((D5/2.2)*500) / (Data!$J$8 + Data!$J$9*C5 + Data!$J$10*C5^2 + Data!$J$11*C5^3 + Data!$J$12*C5^4 + Data!$J$13*C5^5)</f>
-        <v>207.67487661192092</v>
+        <v>204.35422339437085</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6" s="6">
-        <v>67.5</v>
+        <v>75</v>
       </c>
       <c r="D6" s="6">
-        <v>583.1</v>
+        <v>668</v>
       </c>
       <c r="E6" s="4">
         <f t="shared" si="0"/>
-        <v>3.9265993265993266</v>
+        <v>4.0484848484848488</v>
       </c>
       <c r="F6" s="4">
         <f>((D6/2.2)*500) / (Data!$J$8 + Data!$J$9*C6 + Data!$J$10*C6^2 + Data!$J$11*C6^3 + Data!$J$12*C6^4 + Data!$J$13*C6^5)</f>
-        <v>204.35422339437085</v>
+        <v>216.35927101130713</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7" s="6">
-        <v>75</v>
+        <v>82.5</v>
       </c>
       <c r="D7" s="6">
-        <v>668</v>
+        <v>672.4</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" si="0"/>
-        <v>4.0484848484848488</v>
+        <v>3.7046831955922856</v>
       </c>
       <c r="F7" s="4">
         <f>((D7/2.2)*500) / (Data!$J$8 + Data!$J$9*C7 + Data!$J$10*C7^2 + Data!$J$11*C7^3 + Data!$J$12*C7^4 + Data!$J$13*C7^5)</f>
-        <v>216.35927101130713</v>
+        <v>204.74779488917525</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8" s="6">
-        <v>82.5</v>
+        <v>90</v>
       </c>
       <c r="D8" s="6">
-        <v>672.4</v>
+        <v>622.79999999999995</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
-        <v>3.7046831955922856</v>
+        <v>3.1454545454545446</v>
       </c>
       <c r="F8" s="4">
         <f>((D8/2.2)*500) / (Data!$J$8 + Data!$J$9*C8 + Data!$J$10*C8^2 + Data!$J$11*C8^3 + Data!$J$12*C8^4 + Data!$J$13*C8^5)</f>
-        <v>204.74779488917525</v>
+        <v>180.72355943834526</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9" s="6">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D9" s="6">
-        <v>622.79999999999995</v>
+        <v>744.1</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
-        <v>3.1454545454545446</v>
+        <v>3.3822727272727269</v>
       </c>
       <c r="F9" s="4">
         <f>((D9/2.2)*500) / (Data!$J$8 + Data!$J$9*C9 + Data!$J$10*C9^2 + Data!$J$11*C9^3 + Data!$J$12*C9^4 + Data!$J$13*C9^5)</f>
-        <v>180.72355943834526</v>
+        <v>205.84142200260862</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10" s="6">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D10" s="6">
-        <v>744.1</v>
+        <v>815.7</v>
       </c>
       <c r="E10" s="4">
         <f t="shared" si="0"/>
-        <v>3.3822727272727269</v>
+        <v>3.3706611570247933</v>
       </c>
       <c r="F10" s="4">
         <f>((D10/2.2)*500) / (Data!$J$8 + Data!$J$9*C10 + Data!$J$10*C10^2 + Data!$J$11*C10^3 + Data!$J$12*C10^4 + Data!$J$13*C10^5)</f>
-        <v>205.84142200260862</v>
+        <v>218.19723437576295</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11" s="6">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="D11" s="6">
-        <v>815.7</v>
+        <v>853.2</v>
       </c>
       <c r="E11" s="4">
         <f t="shared" si="0"/>
-        <v>3.3706611570247933</v>
+        <v>3.1025454545454547</v>
       </c>
       <c r="F11" s="4">
         <f>((D11/2.2)*500) / (Data!$J$8 + Data!$J$9*C11 + Data!$J$10*C11^2 + Data!$J$11*C11^3 + Data!$J$12*C11^4 + Data!$J$13*C11^5)</f>
-        <v>218.19723437576295</v>
+        <v>220.99619667120635</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12" s="6">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="D12" s="6">
-        <v>853.2</v>
+        <v>705.5</v>
       </c>
       <c r="E12" s="4">
         <f t="shared" si="0"/>
-        <v>3.1025454545454547</v>
+        <v>2.2905844155844157</v>
       </c>
       <c r="F12" s="4">
         <f>((D12/2.2)*500) / (Data!$J$8 + Data!$J$9*C12 + Data!$J$10*C12^2 + Data!$J$11*C12^3 + Data!$J$12*C12^4 + Data!$J$13*C12^5)</f>
-        <v>220.99619667120635</v>
+        <v>179.19914100240959</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C13" s="6">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="D13" s="6">
-        <v>705.5</v>
+        <v>1080.3</v>
       </c>
       <c r="E13" s="4">
         <f t="shared" si="0"/>
-        <v>2.2905844155844157</v>
+        <v>3.2736363636363635</v>
       </c>
       <c r="F13" s="4">
         <f>((D13/2.2)*500) / (Data!$J$8 + Data!$J$9*C13 + Data!$J$10*C13^2 + Data!$J$11*C13^3 + Data!$J$12*C13^4 + Data!$J$13*C13^5)</f>
-        <v>179.19914100240959</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B14" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="6">
-        <v>150</v>
-      </c>
-      <c r="D14" s="6">
-        <v>1080.3</v>
-      </c>
-      <c r="E14" s="4">
-        <f t="shared" si="0"/>
-        <v>3.2736363636363635</v>
-      </c>
-      <c r="F14" s="4">
-        <f>((D14/2.2)*500) / (Data!$J$8 + Data!$J$9*C14 + Data!$J$10*C14^2 + Data!$J$11*C14^3 + Data!$J$12*C14^4 + Data!$J$13*C14^5)</f>
         <v>271.69320263371651</v>
       </c>
     </row>
@@ -10327,256 +10327,256 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AB22E42-A8CB-414A-9166-81C7E5F1C97D}">
-  <dimension ref="B2:F14"/>
+  <dimension ref="B1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F2"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>15</v>
+      <c r="B2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="6">
+        <v>52</v>
+      </c>
+      <c r="D2" s="6">
+        <v>220.5</v>
+      </c>
+      <c r="E2" s="4">
+        <f>D2/(C2*2.2)</f>
+        <v>1.9274475524475523</v>
+      </c>
+      <c r="F2" s="4">
+        <f>((D2/2.2)*500) / (Data!$J$8 + Data!$J$9*C2 + Data!$J$10*C2^2 + Data!$J$11*C2^3 + Data!$J$12*C2^4 + Data!$J$13*C2^5)</f>
+        <v>98.350865072093697</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C3" s="6">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D3" s="6">
-        <v>220.5</v>
+        <v>253.5</v>
       </c>
       <c r="E3" s="4">
-        <f>D3/(C3*2.2)</f>
-        <v>1.9274475524475523</v>
+        <f t="shared" ref="E3:E13" si="0">D3/(C3*2.2)</f>
+        <v>2.0576298701298699</v>
       </c>
       <c r="F3" s="4">
         <f>((D3/2.2)*500) / (Data!$J$8 + Data!$J$9*C3 + Data!$J$10*C3^2 + Data!$J$11*C3^3 + Data!$J$12*C3^4 + Data!$J$13*C3^5)</f>
-        <v>98.350865072093697</v>
+        <v>104.8969487146903</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C4" s="6">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D4" s="6">
-        <v>253.5</v>
+        <v>335.1</v>
       </c>
       <c r="E4" s="4">
-        <f t="shared" ref="E4:E14" si="0">D4/(C4*2.2)</f>
-        <v>2.0576298701298699</v>
+        <f t="shared" si="0"/>
+        <v>2.538636363636364</v>
       </c>
       <c r="F4" s="4">
         <f>((D4/2.2)*500) / (Data!$J$8 + Data!$J$9*C4 + Data!$J$10*C4^2 + Data!$J$11*C4^3 + Data!$J$12*C4^4 + Data!$J$13*C4^5)</f>
-        <v>104.8969487146903</v>
+        <v>129.90825303836979</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C5" s="6">
-        <v>60</v>
+        <v>67.5</v>
       </c>
       <c r="D5" s="6">
-        <v>335.1</v>
+        <v>392.4</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" si="0"/>
-        <v>2.538636363636364</v>
+        <v>2.6424242424242421</v>
       </c>
       <c r="F5" s="4">
         <f>((D5/2.2)*500) / (Data!$J$8 + Data!$J$9*C5 + Data!$J$10*C5^2 + Data!$J$11*C5^3 + Data!$J$12*C5^4 + Data!$J$13*C5^5)</f>
-        <v>129.90825303836979</v>
+        <v>137.52117520142531</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6" s="6">
-        <v>67.5</v>
+        <v>75</v>
       </c>
       <c r="D6" s="6">
-        <v>392.4</v>
+        <v>438.7</v>
       </c>
       <c r="E6" s="4">
         <f t="shared" si="0"/>
-        <v>2.6424242424242421</v>
+        <v>2.6587878787878787</v>
       </c>
       <c r="F6" s="4">
         <f>((D6/2.2)*500) / (Data!$J$8 + Data!$J$9*C6 + Data!$J$10*C6^2 + Data!$J$11*C6^3 + Data!$J$12*C6^4 + Data!$J$13*C6^5)</f>
-        <v>137.52117520142531</v>
+        <v>142.09103621655751</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7" s="6">
-        <v>75</v>
+        <v>82.5</v>
       </c>
       <c r="D7" s="6">
-        <v>438.7</v>
+        <v>440.9</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" si="0"/>
-        <v>2.6587878787878787</v>
+        <v>2.4292011019283741</v>
       </c>
       <c r="F7" s="4">
         <f>((D7/2.2)*500) / (Data!$J$8 + Data!$J$9*C7 + Data!$J$10*C7^2 + Data!$J$11*C7^3 + Data!$J$12*C7^4 + Data!$J$13*C7^5)</f>
-        <v>142.09103621655751</v>
+        <v>134.25535807054931</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="C8" s="6">
-        <v>82.5</v>
+        <v>90</v>
       </c>
       <c r="D8" s="6">
-        <v>440.9</v>
+        <v>474</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
-        <v>2.4292011019283741</v>
+        <v>2.3939393939393936</v>
       </c>
       <c r="F8" s="4">
         <f>((D8/2.2)*500) / (Data!$J$8 + Data!$J$9*C8 + Data!$J$10*C8^2 + Data!$J$11*C8^3 + Data!$J$12*C8^4 + Data!$J$13*C8^5)</f>
-        <v>134.25535807054931</v>
+        <v>137.54490554556145</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C9" s="6">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D9" s="6">
-        <v>474</v>
+        <v>524.70000000000005</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
-        <v>2.3939393939393936</v>
+        <v>2.3849999999999998</v>
       </c>
       <c r="F9" s="4">
         <f>((D9/2.2)*500) / (Data!$J$8 + Data!$J$9*C9 + Data!$J$10*C9^2 + Data!$J$11*C9^3 + Data!$J$12*C9^4 + Data!$J$13*C9^5)</f>
-        <v>137.54490554556145</v>
+        <v>145.14849364973625</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C10" s="6">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D10" s="6">
-        <v>524.70000000000005</v>
+        <v>584.20000000000005</v>
       </c>
       <c r="E10" s="4">
         <f t="shared" si="0"/>
-        <v>2.3849999999999998</v>
+        <v>2.4140495867768594</v>
       </c>
       <c r="F10" s="4">
         <f>((D10/2.2)*500) / (Data!$J$8 + Data!$J$9*C10 + Data!$J$10*C10^2 + Data!$J$11*C10^3 + Data!$J$12*C10^4 + Data!$J$13*C10^5)</f>
-        <v>145.14849364973625</v>
+        <v>156.27169832330605</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C11" s="6">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="D11" s="6">
-        <v>584.20000000000005</v>
+        <v>501.6</v>
       </c>
       <c r="E11" s="4">
         <f t="shared" si="0"/>
-        <v>2.4140495867768594</v>
+        <v>1.8240000000000001</v>
       </c>
       <c r="F11" s="4">
         <f>((D11/2.2)*500) / (Data!$J$8 + Data!$J$9*C11 + Data!$J$10*C11^2 + Data!$J$11*C11^3 + Data!$J$12*C11^4 + Data!$J$13*C11^5)</f>
-        <v>156.27169832330605</v>
+        <v>129.92462757885269</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C12" s="6">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="D12" s="6">
-        <v>501.6</v>
+        <v>463</v>
       </c>
       <c r="E12" s="4">
         <f t="shared" si="0"/>
-        <v>1.8240000000000001</v>
+        <v>1.5032467532467533</v>
       </c>
       <c r="F12" s="4">
         <f>((D12/2.2)*500) / (Data!$J$8 + Data!$J$9*C12 + Data!$J$10*C12^2 + Data!$J$11*C12^3 + Data!$J$12*C12^4 + Data!$J$13*C12^5)</f>
-        <v>129.92462757885269</v>
+        <v>117.60340508024898</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C13" s="6">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="D13" s="6">
-        <v>463</v>
+        <v>619.5</v>
       </c>
       <c r="E13" s="4">
         <f t="shared" si="0"/>
-        <v>1.5032467532467533</v>
+        <v>1.8772727272727272</v>
       </c>
       <c r="F13" s="4">
         <f>((D13/2.2)*500) / (Data!$J$8 + Data!$J$9*C13 + Data!$J$10*C13^2 + Data!$J$11*C13^3 + Data!$J$12*C13^4 + Data!$J$13*C13^5)</f>
-        <v>117.60340508024898</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B14" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="6">
-        <v>150</v>
-      </c>
-      <c r="D14" s="6">
-        <v>619.5</v>
-      </c>
-      <c r="E14" s="4">
-        <f t="shared" si="0"/>
-        <v>1.8772727272727272</v>
-      </c>
-      <c r="F14" s="4">
-        <f>((D14/2.2)*500) / (Data!$J$8 + Data!$J$9*C14 + Data!$J$10*C14^2 + Data!$J$11*C14^3 + Data!$J$12*C14^4 + Data!$J$13*C14^5)</f>
         <v>155.80296124371691</v>
       </c>
     </row>
@@ -10587,162 +10587,181 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD8C4994-989E-4DB6-ABDE-D8C29797DC9B}">
-  <dimension ref="B2:F14"/>
+  <dimension ref="B1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>15</v>
+        <v>43</v>
+      </c>
+      <c r="C2" s="7">
+        <v>52</v>
+      </c>
+      <c r="D2" s="7">
+        <v>253.5</v>
+      </c>
+      <c r="E2" s="4">
+        <f>D2/(C2*2.2)</f>
+        <v>2.2159090909090908</v>
+      </c>
+      <c r="F2" s="4">
+        <f>((D2/2.2)*500) / (Data!$J$8 + Data!$J$9*C2 + Data!$J$10*C2^2 + Data!$J$11*C2^3 + Data!$J$12*C2^4 + Data!$J$13*C2^5)</f>
+        <v>113.07004215771317</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C3" s="7">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D3" s="7">
-        <v>253.5</v>
+        <v>512.6</v>
       </c>
       <c r="E3" s="4">
-        <f>D3/(C3*2.2)</f>
-        <v>2.2159090909090908</v>
+        <f t="shared" ref="E3:E13" si="0">D3/(C3*2.2)</f>
+        <v>4.1607142857142856</v>
       </c>
       <c r="F3" s="4">
         <f>((D3/2.2)*500) / (Data!$J$8 + Data!$J$9*C3 + Data!$J$10*C3^2 + Data!$J$11*C3^3 + Data!$J$12*C3^4 + Data!$J$13*C3^5)</f>
-        <v>113.07004215771317</v>
+        <v>212.11114757850197</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4" s="7" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="C4" s="7">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D4" s="7">
-        <v>512.6</v>
+        <v>606.29999999999995</v>
       </c>
       <c r="E4" s="4">
-        <f t="shared" ref="E4:E14" si="0">D4/(C4*2.2)</f>
-        <v>4.1607142857142856</v>
+        <f t="shared" si="0"/>
+        <v>4.5931818181818178</v>
       </c>
       <c r="F4" s="4">
         <f>((D4/2.2)*500) / (Data!$J$8 + Data!$J$9*C4 + Data!$J$10*C4^2 + Data!$J$11*C4^3 + Data!$J$12*C4^4 + Data!$J$13*C4^5)</f>
-        <v>212.11114757850197</v>
+        <v>235.04438620460638</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C5" s="7">
-        <v>60</v>
+        <v>67.5</v>
       </c>
       <c r="D5" s="7">
-        <v>606.29999999999995</v>
+        <v>655.9</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" si="0"/>
-        <v>4.5931818181818178</v>
+        <v>4.4168350168350168</v>
       </c>
       <c r="F5" s="4">
         <f>((D5/2.2)*500) / (Data!$J$8 + Data!$J$9*C5 + Data!$J$10*C5^2 + Data!$J$11*C5^3 + Data!$J$12*C5^4 + Data!$J$13*C5^5)</f>
-        <v>235.04438620460638</v>
+        <v>229.86783591899814</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" s="7" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="C6" s="7">
-        <v>67.5</v>
+        <v>75</v>
       </c>
       <c r="D6" s="7">
-        <v>655.9</v>
+        <v>750.7</v>
       </c>
       <c r="E6" s="4">
         <f t="shared" si="0"/>
-        <v>4.4168350168350168</v>
+        <v>4.5496969696969698</v>
       </c>
       <c r="F6" s="4">
         <f>((D6/2.2)*500) / (Data!$J$8 + Data!$J$9*C6 + Data!$J$10*C6^2 + Data!$J$11*C6^3 + Data!$J$12*C6^4 + Data!$J$13*C6^5)</f>
-        <v>229.86783591899814</v>
+        <v>243.14506698830581</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7" s="7" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="C7" s="7">
-        <v>75</v>
+        <v>82.5</v>
       </c>
       <c r="D7" s="7">
-        <v>750.7</v>
+        <v>771.6</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" si="0"/>
-        <v>4.5496969696969698</v>
+        <v>4.2512396694214871</v>
       </c>
       <c r="F7" s="4">
         <f>((D7/2.2)*500) / (Data!$J$8 + Data!$J$9*C7 + Data!$J$10*C7^2 + Data!$J$11*C7^3 + Data!$J$12*C7^4 + Data!$J$13*C7^5)</f>
-        <v>243.14506698830581</v>
+        <v>234.95448919763177</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C8" s="7">
-        <v>82.5</v>
+        <v>90</v>
       </c>
       <c r="D8" s="7">
-        <v>771.6</v>
+        <v>406.6</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
-        <v>4.2512396694214871</v>
+        <v>2.0535353535353535</v>
       </c>
       <c r="F8" s="4">
         <f>((D8/2.2)*500) / (Data!$J$8 + Data!$J$9*C8 + Data!$J$10*C8^2 + Data!$J$11*C8^3 + Data!$J$12*C8^4 + Data!$J$13*C8^5)</f>
-        <v>234.95448919763177</v>
+        <v>117.98683247853435</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B9" s="7" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="C9" s="7">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D9" s="7">
-        <v>406.6</v>
+        <v>844.4</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
-        <v>2.0535353535353535</v>
+        <v>3.8381818181818175</v>
       </c>
       <c r="F9" s="4">
         <f>((D9/2.2)*500) / (Data!$J$8 + Data!$J$9*C9 + Data!$J$10*C9^2 + Data!$J$11*C9^3 + Data!$J$12*C9^4 + Data!$J$13*C9^5)</f>
-        <v>117.98683247853435</v>
+        <v>233.58755105362548</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.2">
@@ -10750,93 +10769,74 @@
         <v>9</v>
       </c>
       <c r="C10" s="7">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D10" s="7">
-        <v>844.4</v>
+        <v>837.8</v>
       </c>
       <c r="E10" s="4">
         <f t="shared" si="0"/>
-        <v>3.8381818181818175</v>
+        <v>3.4619834710743795</v>
       </c>
       <c r="F10" s="4">
         <f>((D10/2.2)*500) / (Data!$J$8 + Data!$J$9*C10 + Data!$J$10*C10^2 + Data!$J$11*C10^3 + Data!$J$12*C10^4 + Data!$J$13*C10^5)</f>
-        <v>233.58755105362548</v>
+        <v>224.10891621921564</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B11" s="7" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="C11" s="7">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="D11" s="7">
-        <v>837.8</v>
+        <v>843.3</v>
       </c>
       <c r="E11" s="4">
         <f t="shared" si="0"/>
-        <v>3.4619834710743795</v>
+        <v>3.0665454545454542</v>
       </c>
       <c r="F11" s="4">
         <f>((D11/2.2)*500) / (Data!$J$8 + Data!$J$9*C11 + Data!$J$10*C11^2 + Data!$J$11*C11^3 + Data!$J$12*C11^4 + Data!$J$13*C11^5)</f>
-        <v>224.10891621921564</v>
+        <v>218.43189481109738</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B12" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C12" s="7">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="D12" s="7">
-        <v>843.3</v>
+        <v>705.5</v>
       </c>
       <c r="E12" s="4">
         <f t="shared" si="0"/>
-        <v>3.0665454545454542</v>
+        <v>2.2905844155844157</v>
       </c>
       <c r="F12" s="4">
         <f>((D12/2.2)*500) / (Data!$J$8 + Data!$J$9*C12 + Data!$J$10*C12^2 + Data!$J$11*C12^3 + Data!$J$12*C12^4 + Data!$J$13*C12^5)</f>
-        <v>218.43189481109738</v>
+        <v>179.19914100240959</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B13" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" s="7">
-        <v>140</v>
-      </c>
-      <c r="D13" s="7">
-        <v>705.5</v>
+      <c r="B13" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="6">
+        <v>150</v>
+      </c>
+      <c r="D13" s="6">
+        <v>881.8</v>
       </c>
       <c r="E13" s="4">
         <f t="shared" si="0"/>
-        <v>2.2905844155844157</v>
+        <v>2.6721212121212119</v>
       </c>
       <c r="F13" s="4">
         <f>((D13/2.2)*500) / (Data!$J$8 + Data!$J$9*C13 + Data!$J$10*C13^2 + Data!$J$11*C13^3 + Data!$J$12*C13^4 + Data!$J$13*C13^5)</f>
-        <v>179.19914100240959</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B14" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C14" s="6">
-        <v>150</v>
-      </c>
-      <c r="D14" s="6">
-        <v>881.8</v>
-      </c>
-      <c r="E14" s="4">
-        <f t="shared" si="0"/>
-        <v>2.6721212121212119</v>
-      </c>
-      <c r="F14" s="4">
-        <f>((D14/2.2)*500) / (Data!$J$8 + Data!$J$9*C14 + Data!$J$10*C14^2 + Data!$J$11*C14^3 + Data!$J$12*C14^4 + Data!$J$13*C14^5)</f>
         <v>221.77086557660948</v>
       </c>
     </row>
@@ -10847,162 +10847,181 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B562DC9-99AB-4A23-98BC-E911B85042EB}">
-  <dimension ref="B2:F14"/>
+  <dimension ref="B1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F2"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>15</v>
+      <c r="B2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6">
+        <v>52</v>
+      </c>
+      <c r="D2" s="6">
+        <v>788.2</v>
+      </c>
+      <c r="E2" s="4">
+        <f>D2/(C2*2.2)</f>
+        <v>6.88986013986014</v>
+      </c>
+      <c r="F2" s="4">
+        <f>((D2/2.2)*500) / (Data!$J$8 + Data!$J$9*C2 + Data!$J$10*C2^2 + Data!$J$11*C2^3 + Data!$J$12*C2^4 + Data!$J$13*C2^5)</f>
+        <v>351.56531451167461</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" s="6">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D3" s="6">
-        <v>788.2</v>
+        <v>1162.9000000000001</v>
       </c>
       <c r="E3" s="4">
-        <f>D3/(C3*2.2)</f>
-        <v>6.88986013986014</v>
+        <f t="shared" ref="E3:E13" si="0">D3/(C3*2.2)</f>
+        <v>9.4391233766233764</v>
       </c>
       <c r="F3" s="4">
         <f>((D3/2.2)*500) / (Data!$J$8 + Data!$J$9*C3 + Data!$J$10*C3^2 + Data!$J$11*C3^3 + Data!$J$12*C3^4 + Data!$J$13*C3^5)</f>
-        <v>351.56531451167461</v>
+        <v>481.20182114522038</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
-        <v>2</v>
+        <v>44</v>
       </c>
       <c r="C4" s="6">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D4" s="6">
-        <v>1162.9000000000001</v>
+        <v>1372.4</v>
       </c>
       <c r="E4" s="4">
-        <f t="shared" ref="E4:E14" si="0">D4/(C4*2.2)</f>
-        <v>9.4391233766233764</v>
+        <f t="shared" si="0"/>
+        <v>10.396969696969698</v>
       </c>
       <c r="F4" s="4">
         <f>((D4/2.2)*500) / (Data!$J$8 + Data!$J$9*C4 + Data!$J$10*C4^2 + Data!$J$11*C4^3 + Data!$J$12*C4^4 + Data!$J$13*C4^5)</f>
-        <v>481.20182114522038</v>
+        <v>532.03845559492299</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C5" s="6">
-        <v>60</v>
+        <v>67.5</v>
       </c>
       <c r="D5" s="6">
-        <v>1372.4</v>
+        <v>1555.4</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" si="0"/>
-        <v>10.396969696969698</v>
+        <v>10.474074074074075</v>
       </c>
       <c r="F5" s="4">
         <f>((D5/2.2)*500) / (Data!$J$8 + Data!$J$9*C5 + Data!$J$10*C5^2 + Data!$J$11*C5^3 + Data!$J$12*C5^4 + Data!$J$13*C5^5)</f>
-        <v>532.03845559492299</v>
+        <v>545.10814451655699</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="C6" s="6">
-        <v>67.5</v>
+        <v>75</v>
       </c>
       <c r="D6" s="6">
-        <v>1555.4</v>
+        <v>1848.6</v>
       </c>
       <c r="E6" s="4">
         <f t="shared" si="0"/>
-        <v>10.474074074074075</v>
+        <v>11.203636363636363</v>
       </c>
       <c r="F6" s="4">
         <f>((D6/2.2)*500) / (Data!$J$8 + Data!$J$9*C6 + Data!$J$10*C6^2 + Data!$J$11*C6^3 + Data!$J$12*C6^4 + Data!$J$13*C6^5)</f>
-        <v>545.10814451655699</v>
+        <v>598.74513232260824</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7" s="6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7" s="6">
-        <v>75</v>
+        <v>82.5</v>
       </c>
       <c r="D7" s="6">
-        <v>1848.6</v>
+        <v>1802.3</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" si="0"/>
-        <v>11.203636363636363</v>
+        <v>9.930027548209365</v>
       </c>
       <c r="F7" s="4">
         <f>((D7/2.2)*500) / (Data!$J$8 + Data!$J$9*C7 + Data!$J$10*C7^2 + Data!$J$11*C7^3 + Data!$J$12*C7^4 + Data!$J$13*C7^5)</f>
-        <v>598.74513232260824</v>
+        <v>548.80569709809708</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="C8" s="6">
-        <v>82.5</v>
+        <v>90</v>
       </c>
       <c r="D8" s="6">
-        <v>1802.3</v>
+        <v>1686.5</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
-        <v>9.930027548209365</v>
+        <v>8.5176767676767664</v>
       </c>
       <c r="F8" s="4">
         <f>((D8/2.2)*500) / (Data!$J$8 + Data!$J$9*C8 + Data!$J$10*C8^2 + Data!$J$11*C8^3 + Data!$J$12*C8^4 + Data!$J$13*C8^5)</f>
-        <v>548.80569709809708</v>
+        <v>489.38709536411261</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>53</v>
+        <v>9</v>
       </c>
       <c r="C9" s="6">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D9" s="6">
-        <v>1686.5</v>
+        <v>1943.4</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
-        <v>8.5176767676767664</v>
+        <v>8.8336363636363622</v>
       </c>
       <c r="F9" s="4">
         <f>((D9/2.2)*500) / (Data!$J$8 + Data!$J$9*C9 + Data!$J$10*C9^2 + Data!$J$11*C9^3 + Data!$J$12*C9^4 + Data!$J$13*C9^5)</f>
-        <v>489.38709536411261</v>
+        <v>537.60545561062975</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.2">
@@ -11010,93 +11029,74 @@
         <v>9</v>
       </c>
       <c r="C10" s="6">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D10" s="6">
-        <v>1943.4</v>
+        <v>2105.4</v>
       </c>
       <c r="E10" s="4">
         <f t="shared" si="0"/>
-        <v>8.8336363636363622</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="F10" s="4">
         <f>((D10/2.2)*500) / (Data!$J$8 + Data!$J$9*C10 + Data!$J$10*C10^2 + Data!$J$11*C10^3 + Data!$J$12*C10^4 + Data!$J$13*C10^5)</f>
-        <v>537.60545561062975</v>
+        <v>563.18800693236653</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11" s="6">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="D11" s="6">
-        <v>2105.4</v>
+        <v>2157.1999999999998</v>
       </c>
       <c r="E11" s="4">
         <f t="shared" si="0"/>
-        <v>8.6999999999999993</v>
+        <v>7.844363636363636</v>
       </c>
       <c r="F11" s="4">
         <f>((D11/2.2)*500) / (Data!$J$8 + Data!$J$9*C11 + Data!$J$10*C11^2 + Data!$J$11*C11^3 + Data!$J$12*C11^4 + Data!$J$13*C11^5)</f>
-        <v>563.18800693236653</v>
+        <v>558.75878511383758</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="C12" s="6">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="D12" s="6">
-        <v>2157.1999999999998</v>
+        <v>1791.3</v>
       </c>
       <c r="E12" s="4">
         <f t="shared" si="0"/>
-        <v>7.844363636363636</v>
+        <v>5.8159090909090905</v>
       </c>
       <c r="F12" s="4">
         <f>((D12/2.2)*500) / (Data!$J$8 + Data!$J$9*C12 + Data!$J$10*C12^2 + Data!$J$11*C12^3 + Data!$J$12*C12^4 + Data!$J$13*C12^5)</f>
-        <v>558.75878511383758</v>
+        <v>454.99563611285095</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="C13" s="6">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="D13" s="6">
-        <v>1791.3</v>
+        <v>2452.6</v>
       </c>
       <c r="E13" s="4">
         <f t="shared" si="0"/>
-        <v>5.8159090909090905</v>
+        <v>7.4321212121212117</v>
       </c>
       <c r="F13" s="4">
         <f>((D13/2.2)*500) / (Data!$J$8 + Data!$J$9*C13 + Data!$J$10*C13^2 + Data!$J$11*C13^3 + Data!$J$12*C13^4 + Data!$J$13*C13^5)</f>
-        <v>454.99563611285095</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B14" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="6">
-        <v>150</v>
-      </c>
-      <c r="D14" s="6">
-        <v>2452.6</v>
-      </c>
-      <c r="E14" s="4">
-        <f t="shared" si="0"/>
-        <v>7.4321212121212117</v>
-      </c>
-      <c r="F14" s="4">
-        <f>((D14/2.2)*500) / (Data!$J$8 + Data!$J$9*C14 + Data!$J$10*C14^2 + Data!$J$11*C14^3 + Data!$J$12*C14^4 + Data!$J$13*C14^5)</f>
         <v>616.82379781491534</v>
       </c>
     </row>
@@ -11107,105 +11107,124 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{725CA7E6-274F-44F9-9097-F9A973F00E58}">
-  <dimension ref="B2:F13"/>
+  <dimension ref="B1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F2"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>15</v>
+      <c r="B2" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="6">
+        <v>44</v>
+      </c>
+      <c r="D2" s="6">
+        <v>187.4</v>
+      </c>
+      <c r="E2" s="4">
+        <f>D2/(C2*2.2)</f>
+        <v>1.9359504132231404</v>
+      </c>
+      <c r="F2" s="4">
+        <f>((D2/2.2)*500) / (Data!$J$15 + Data!$J$16*C2 + Data!$J$17*C2^2 +Data!$J$18*C2^3 + Data!$J$19*C2^4 + Data!$J$20*C2^5)</f>
+        <v>119.94201818783097</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C3" s="6">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D3" s="6">
-        <v>187.4</v>
+        <v>315.3</v>
       </c>
       <c r="E3" s="4">
-        <f>D3/(C3*2.2)</f>
-        <v>1.9359504132231404</v>
+        <f t="shared" ref="E3:E12" si="0">D3/(C3*2.2)</f>
+        <v>2.9857954545454546</v>
       </c>
       <c r="F3" s="4">
         <f>((D3/2.2)*500) / (Data!$J$15 + Data!$J$16*C3 + Data!$J$17*C3^2 +Data!$J$18*C3^3 + Data!$J$19*C3^4 + Data!$J$20*C3^5)</f>
-        <v>119.94201818783097</v>
+        <v>189.81352833754997</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C4" s="6">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D4" s="6">
-        <v>315.3</v>
+        <v>345</v>
       </c>
       <c r="E4" s="4">
-        <f t="shared" ref="E4:E13" si="0">D4/(C4*2.2)</f>
-        <v>2.9857954545454546</v>
+        <f t="shared" si="0"/>
+        <v>3.0157342657342654</v>
       </c>
       <c r="F4" s="4">
         <f>((D4/2.2)*500) / (Data!$J$15 + Data!$J$16*C4 + Data!$J$17*C4^2 +Data!$J$18*C4^3 + Data!$J$19*C4^4 + Data!$J$20*C4^5)</f>
-        <v>189.81352833754997</v>
+        <v>195.4953460697283</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C5" s="6">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D5" s="6">
-        <v>345</v>
+        <v>377</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" si="0"/>
-        <v>3.0157342657342654</v>
+        <v>3.0600649350649345</v>
       </c>
       <c r="F5" s="4">
         <f>((D5/2.2)*500) / (Data!$J$15 + Data!$J$16*C5 + Data!$J$17*C5^2 +Data!$J$18*C5^3 + Data!$J$19*C5^4 + Data!$J$20*C5^5)</f>
-        <v>195.4953460697283</v>
+        <v>201.62732958488559</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="6">
         <v>60</v>
       </c>
-      <c r="C6" s="6">
-        <v>56</v>
-      </c>
       <c r="D6" s="6">
-        <v>377</v>
+        <v>392.4</v>
       </c>
       <c r="E6" s="4">
         <f t="shared" si="0"/>
-        <v>3.0600649350649345</v>
+        <v>2.9727272727272727</v>
       </c>
       <c r="F6" s="4">
         <f>((D6/2.2)*500) / (Data!$J$15 + Data!$J$16*C6 + Data!$J$17*C6^2 +Data!$J$18*C6^3 + Data!$J$19*C6^4 + Data!$J$20*C6^5)</f>
-        <v>201.62732958488559</v>
+        <v>198.85527721136046</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
@@ -11213,131 +11232,112 @@
         <v>61</v>
       </c>
       <c r="C7" s="6">
-        <v>60</v>
+        <v>67.5</v>
       </c>
       <c r="D7" s="6">
-        <v>392.4</v>
+        <v>413.4</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" si="0"/>
-        <v>2.9727272727272727</v>
+        <v>2.7838383838383836</v>
       </c>
       <c r="F7" s="4">
         <f>((D7/2.2)*500) / (Data!$J$15 + Data!$J$16*C7 + Data!$J$17*C7^2 +Data!$J$18*C7^3 + Data!$J$19*C7^4 + Data!$J$20*C7^5)</f>
-        <v>198.85527721136046</v>
+        <v>191.78404281548936</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C8" s="6">
-        <v>67.5</v>
+        <v>75</v>
       </c>
       <c r="D8" s="6">
-        <v>413.4</v>
+        <v>453</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
-        <v>2.7838383838383836</v>
+        <v>2.7454545454545456</v>
       </c>
       <c r="F8" s="4">
         <f>((D8/2.2)*500) / (Data!$J$15 + Data!$J$16*C8 + Data!$J$17*C8^2 +Data!$J$18*C8^3 + Data!$J$19*C8^4 + Data!$J$20*C8^5)</f>
-        <v>191.78404281548936</v>
+        <v>195.74555326873454</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C9" s="6">
-        <v>75</v>
+        <v>82.5</v>
       </c>
       <c r="D9" s="6">
-        <v>453</v>
+        <v>440.9</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
-        <v>2.7454545454545456</v>
+        <v>2.4292011019283741</v>
       </c>
       <c r="F9" s="4">
         <f>((D9/2.2)*500) / (Data!$J$15 + Data!$J$16*C9 + Data!$J$17*C9^2 +Data!$J$18*C9^3 + Data!$J$19*C9^4 + Data!$J$20*C9^5)</f>
-        <v>195.74555326873454</v>
+        <v>180.36203401468237</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C10" s="6">
-        <v>82.5</v>
+        <v>90</v>
       </c>
       <c r="D10" s="6">
-        <v>440.9</v>
+        <v>564.4</v>
       </c>
       <c r="E10" s="4">
         <f t="shared" si="0"/>
-        <v>2.4292011019283741</v>
+        <v>2.85050505050505</v>
       </c>
       <c r="F10" s="4">
         <f>((D10/2.2)*500) / (Data!$J$15 + Data!$J$16*C10 + Data!$J$17*C10^2 +Data!$J$18*C10^3 + Data!$J$19*C10^4 + Data!$J$20*C10^5)</f>
-        <v>180.36203401468237</v>
+        <v>221.67176442227785</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C11" s="6">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D11" s="6">
-        <v>564.4</v>
+        <v>440.9</v>
       </c>
       <c r="E11" s="4">
         <f t="shared" si="0"/>
-        <v>2.85050505050505</v>
+        <v>2.0040909090909089</v>
       </c>
       <c r="F11" s="4">
         <f>((D11/2.2)*500) / (Data!$J$15 + Data!$J$16*C11 + Data!$J$17*C11^2 +Data!$J$18*C11^3 + Data!$J$19*C11^4 + Data!$J$20*C11^5)</f>
-        <v>221.67176442227785</v>
+        <v>166.85726561330216</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C12" s="6">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D12" s="6">
-        <v>440.9</v>
+        <v>608.5</v>
       </c>
       <c r="E12" s="4">
         <f t="shared" si="0"/>
-        <v>2.0040909090909089</v>
+        <v>2.5144628099173549</v>
       </c>
       <c r="F12" s="4">
         <f>((D12/2.2)*500) / (Data!$J$15 + Data!$J$16*C12 + Data!$J$17*C12^2 +Data!$J$18*C12^3 + Data!$J$19*C12^4 + Data!$J$20*C12^5)</f>
-        <v>166.85726561330216</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B13" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C13" s="6">
-        <v>110</v>
-      </c>
-      <c r="D13" s="6">
-        <v>608.5</v>
-      </c>
-      <c r="E13" s="4">
-        <f t="shared" si="0"/>
-        <v>2.5144628099173549</v>
-      </c>
-      <c r="F13" s="4">
-        <f>((D13/2.2)*500) / (Data!$J$15 + Data!$J$16*C13 + Data!$J$17*C13^2 +Data!$J$18*C13^3 + Data!$J$19*C13^4 + Data!$J$20*C13^5)</f>
         <v>224.88703643914945</v>
       </c>
     </row>
@@ -11348,105 +11348,124 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D18C3D7B-83D2-4907-84B4-9FEDFAAB16BD}">
-  <dimension ref="B2:F13"/>
+  <dimension ref="B1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F2"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>15</v>
+      <c r="B2" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="6">
+        <v>44</v>
+      </c>
+      <c r="D2" s="6">
+        <v>137.80000000000001</v>
+      </c>
+      <c r="E2" s="4">
+        <f>D2/(C2*2.2)</f>
+        <v>1.4235537190082643</v>
+      </c>
+      <c r="F2" s="4">
+        <f>((D2/2.2)*500) / (Data!$J$15 + Data!$J$16*C2 + Data!$J$17*C2^2 + Data!$J$18*C2^3 + Data!$J$19*C2^4 + Data!$J$20*C2^5)</f>
+        <v>88.19642532701765</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="C3" s="6">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D3" s="6">
-        <v>137.80000000000001</v>
+        <v>198.4</v>
       </c>
       <c r="E3" s="4">
-        <f>D3/(C3*2.2)</f>
-        <v>1.4235537190082643</v>
+        <f t="shared" ref="E3:E12" si="0">D3/(C3*2.2)</f>
+        <v>1.8787878787878787</v>
       </c>
       <c r="F3" s="4">
         <f>((D3/2.2)*500) / (Data!$J$15 + Data!$J$16*C3 + Data!$J$17*C3^2 + Data!$J$18*C3^3 + Data!$J$19*C3^4 + Data!$J$20*C3^5)</f>
-        <v>88.19642532701765</v>
+        <v>119.43864263295245</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C4" s="6">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D4" s="6">
-        <v>198.4</v>
+        <v>237</v>
       </c>
       <c r="E4" s="4">
-        <f t="shared" ref="E4:E13" si="0">D4/(C4*2.2)</f>
-        <v>1.8787878787878787</v>
+        <f t="shared" si="0"/>
+        <v>2.0716783216783217</v>
       </c>
       <c r="F4" s="4">
         <f>((D4/2.2)*500) / (Data!$J$15 + Data!$J$16*C4 + Data!$J$17*C4^2 + Data!$J$18*C4^3 + Data!$J$19*C4^4 + Data!$J$20*C4^5)</f>
-        <v>119.43864263295245</v>
+        <v>134.29680295224813</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C5" s="6">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D5" s="6">
-        <v>237</v>
+        <v>256.8</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" si="0"/>
-        <v>2.0716783216783217</v>
+        <v>2.0844155844155843</v>
       </c>
       <c r="F5" s="4">
         <f>((D5/2.2)*500) / (Data!$J$15 + Data!$J$16*C5 + Data!$J$17*C5^2 + Data!$J$18*C5^3 + Data!$J$19*C5^4 + Data!$J$20*C5^5)</f>
-        <v>134.29680295224813</v>
+        <v>137.34190513898838</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C6" s="6">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D6" s="6">
-        <v>256.8</v>
+        <v>300.89999999999998</v>
       </c>
       <c r="E6" s="4">
         <f t="shared" si="0"/>
-        <v>2.0844155844155843</v>
+        <v>2.2795454545454543</v>
       </c>
       <c r="F6" s="4">
         <f>((D6/2.2)*500) / (Data!$J$15 + Data!$J$16*C6 + Data!$J$17*C6^2 + Data!$J$18*C6^3 + Data!$J$19*C6^4 + Data!$J$20*C6^5)</f>
-        <v>137.34190513898838</v>
+        <v>152.48611853439948</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
@@ -11454,131 +11473,112 @@
         <v>70</v>
       </c>
       <c r="C7" s="6">
-        <v>60</v>
+        <v>67.5</v>
       </c>
       <c r="D7" s="6">
-        <v>300.89999999999998</v>
+        <v>317.5</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" si="0"/>
-        <v>2.2795454545454543</v>
+        <v>2.138047138047138</v>
       </c>
       <c r="F7" s="4">
         <f>((D7/2.2)*500) / (Data!$J$15 + Data!$J$16*C7 + Data!$J$17*C7^2 + Data!$J$18*C7^3 + Data!$J$19*C7^4 + Data!$J$20*C7^5)</f>
-        <v>152.48611853439948</v>
+        <v>147.29422736796778</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C8" s="6">
-        <v>67.5</v>
+        <v>75</v>
       </c>
       <c r="D8" s="6">
-        <v>317.5</v>
+        <v>286.60000000000002</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
-        <v>2.138047138047138</v>
+        <v>1.7369696969696971</v>
       </c>
       <c r="F8" s="4">
         <f>((D8/2.2)*500) / (Data!$J$15 + Data!$J$16*C8 + Data!$J$17*C8^2 + Data!$J$18*C8^3 + Data!$J$19*C8^4 + Data!$J$20*C8^5)</f>
-        <v>147.29422736796778</v>
+        <v>123.84255092013095</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C9" s="6">
-        <v>75</v>
+        <v>82.5</v>
       </c>
       <c r="D9" s="6">
-        <v>286.60000000000002</v>
+        <v>253.5</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
-        <v>1.7369696969696971</v>
+        <v>1.3966942148760328</v>
       </c>
       <c r="F9" s="4">
         <f>((D9/2.2)*500) / (Data!$J$15 + Data!$J$16*C9 + Data!$J$17*C9^2 + Data!$J$18*C9^3 + Data!$J$19*C9^4 + Data!$J$20*C9^5)</f>
-        <v>123.84255092013095</v>
+        <v>103.70101071154907</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C10" s="6">
-        <v>82.5</v>
+        <v>90</v>
       </c>
       <c r="D10" s="6">
-        <v>253.5</v>
+        <v>302</v>
       </c>
       <c r="E10" s="4">
         <f t="shared" si="0"/>
-        <v>1.3966942148760328</v>
+        <v>1.5252525252525251</v>
       </c>
       <c r="F10" s="4">
         <f>((D10/2.2)*500) / (Data!$J$15 + Data!$J$16*C10 + Data!$J$17*C10^2 + Data!$J$18*C10^3 + Data!$J$19*C10^4 + Data!$J$20*C10^5)</f>
-        <v>103.70101071154907</v>
+        <v>118.61246076457817</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C11" s="6">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D11" s="6">
-        <v>302</v>
+        <v>259</v>
       </c>
       <c r="E11" s="4">
         <f t="shared" si="0"/>
-        <v>1.5252525252525251</v>
+        <v>1.177272727272727</v>
       </c>
       <c r="F11" s="4">
         <f>((D11/2.2)*500) / (Data!$J$15 + Data!$J$16*C11 + Data!$J$17*C11^2 + Data!$J$18*C11^3 + Data!$J$19*C11^4 + Data!$J$20*C11^5)</f>
-        <v>118.61246076457817</v>
+        <v>98.017763197653139</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="C12" s="6">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D12" s="6">
-        <v>259</v>
+        <v>369.3</v>
       </c>
       <c r="E12" s="4">
         <f t="shared" si="0"/>
-        <v>1.177272727272727</v>
+        <v>1.5260330578512395</v>
       </c>
       <c r="F12" s="4">
         <f>((D12/2.2)*500) / (Data!$J$15 + Data!$J$16*C12 + Data!$J$17*C12^2 + Data!$J$18*C12^3 + Data!$J$19*C12^4 + Data!$J$20*C12^5)</f>
-        <v>98.017763197653139</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B13" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C13" s="6">
-        <v>110</v>
-      </c>
-      <c r="D13" s="6">
-        <v>369.3</v>
-      </c>
-      <c r="E13" s="4">
-        <f t="shared" si="0"/>
-        <v>1.5260330578512395</v>
-      </c>
-      <c r="F13" s="4">
-        <f>((D13/2.2)*500) / (Data!$J$15 + Data!$J$16*C13 + Data!$J$17*C13^2 + Data!$J$18*C13^3 + Data!$J$19*C13^4 + Data!$J$20*C13^5)</f>
         <v>136.48444134260953</v>
       </c>
     </row>

</xml_diff>